<commit_message>
minor edits with text/narrative.
</commit_message>
<xml_diff>
--- a/RDP_institutions.xlsx
+++ b/RDP_institutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lamar/Desktop/DS Projects/RDP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584D8B9A-FB4D-B74B-8114-2BDBF7EFD366}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02EC706-DE95-9946-9578-F4846818CE4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" xr2:uid="{44B40AB0-EA75-5B44-800A-269CA5746C01}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14320" xr2:uid="{44B40AB0-EA75-5B44-800A-269CA5746C01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Institution</t>
   </si>
@@ -154,13 +154,16 @@
   </si>
   <si>
     <t>UNITID</t>
+  </si>
+  <si>
+    <t>University of Wisconsin at Madison</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +198,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -228,6 +237,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC10FD4-3380-5A4C-B785-B3B741B97E63}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,6 +871,14 @@
         <v>230038</v>
       </c>
     </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5">
+        <v>240444</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>